<commit_message>
Housing remote indigenous text changes.
</commit_message>
<xml_diff>
--- a/dashboard_loader/housing_remote_indigenous_uploader/housing_remote_indigenous.xlsx
+++ b/dashboard_loader/housing_remote_indigenous_uploader/housing_remote_indigenous.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t xml:space="preserve">NPARIH capital works progress, number of new houses and refurbishments, by state and territory, 2008-2017 </t>
   </si>
@@ -83,19 +83,121 @@
     <t xml:space="preserve">Desc Body</t>
   </si>
   <si>
-    <t xml:space="preserve">From 2008 to the end of October 2017, the National Partnership on Remote Housing (NPRH) and National Partnership Agreement for Remote Indigenous Housing (NPARIH) delivered a total of 3,444 new houses against the 2018 COAG target of 4,200.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A total of 7,393 refurbishments were delivered, considerably exceeding the 2014 COAG target of 4800.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Each of the jurisdictions that have remained in the NPRH are likely to meet their targets for new builds, with the exception of WA. Nationally, based on current performance, 4,020 new houses are expected to be delivered and 7,557 refurbishments and rebuilds (Commonwealth of Australia 2017).</t>
+    <t xml:space="preserve">New housing construction</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">From 2008 to the end of October 2017, the National Partnership on Remote Housing (NPRH) and National Partnership Agreement for Remote Indigenous Housing (NPARIH) delivered a total of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">3,506</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> new houses against the 2018 COAG target of 4,200. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Each of the jurisdictions that have remained in the NPRH are likely to meet their targets for new builds, with the exception of WA. Nationally, based on current performance, 4,020 new houses are expected to be delivered (Commonwealth of Australia 2017). </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Nationally, this aspect of the benchmark is not on track to be met.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Refurbishment of houses</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">From 2008 to the end of October 2017</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">, a total of 7,393 refurbishments were delivered, considerably exceeding the 2014 COAG target of 4800. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Nationally and for each jurisdiction, this aspect of the benchmark was met.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Victoria and Tasmania exited the NPARIH in 2014 and New South Wales in 2015, and are not part of the NPRH. The ACT is not part of the NPRH.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Victoria and Tasmania exited the NPARIH in 2014 and New South Wales in 2015, and are not part of the NPRH. The ACT is not part of the NPRH. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Tasmania and NSW exited the National Partnership before completing their respective new build targets.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Totals include dwellings built from Commonwealth Own Purpose Expense funding under NPARIH.</t>
@@ -104,13 +206,31 @@
     <t xml:space="preserve">Source</t>
   </si>
   <si>
-    <t xml:space="preserve">State and Territory governments.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">State and Territory governments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">; Department of the Prime Minister and Cabinet.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">References</t>
   </si>
   <si>
-    <t xml:space="preserve">Commonwealth of Australia (2017), Department of the Prime Minister and Cabinet, Remote Housing Review: A review of the National Partnership Agreement on Remote Indigenous Housing and the Remote Housing Strategy (2008-2018)</t>
+    <t xml:space="preserve">Commonwealth of Australia (2017), Department of the Prime Minister and Cabinet, Remote Housing Review: A Review of the National Partnership Agreement on Remote Indigenous Housing and the Remote Housing Strategy (2008–2018)</t>
   </si>
 </sst>
 </file>
@@ -123,7 +243,7 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -187,6 +307,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF00000A"/>
       <name val="Arial"/>
@@ -194,7 +321,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -249,7 +376,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -286,6 +413,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -302,15 +433,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -395,7 +538,7 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="I8" activeCellId="1" sqref="A13:A14 I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -532,11 +675,11 @@
       <c r="G6" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="H6" s="8" t="n">
-        <v>1271</v>
-      </c>
-      <c r="I6" s="8" t="n">
-        <v>3444</v>
+      <c r="H6" s="9" t="n">
+        <v>1333</v>
+      </c>
+      <c r="I6" s="9" t="n">
+        <v>3506</v>
       </c>
       <c r="K6" s="3"/>
     </row>
@@ -571,40 +714,40 @@
       <c r="K7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="9" t="n">
+      <c r="A8" s="10" t="n">
         <v>2018</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="11" t="n">
+      <c r="C8" s="12" t="n">
         <v>310</v>
       </c>
-      <c r="D8" s="11" t="n">
+      <c r="D8" s="12" t="n">
         <v>1141</v>
       </c>
-      <c r="E8" s="11" t="n">
+      <c r="E8" s="12" t="n">
         <v>1012</v>
       </c>
-      <c r="F8" s="11" t="n">
+      <c r="F8" s="12" t="n">
         <v>241</v>
       </c>
-      <c r="G8" s="11" t="n">
+      <c r="G8" s="12" t="n">
         <v>18</v>
       </c>
-      <c r="H8" s="11" t="n">
+      <c r="H8" s="12" t="n">
         <v>1456</v>
       </c>
-      <c r="I8" s="11" t="n">
+      <c r="I8" s="12" t="n">
         <v>4200</v>
       </c>
       <c r="K8" s="3"/>
     </row>
     <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="n">
+      <c r="A9" s="10" t="n">
         <v>2014</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="0" t="n">
@@ -648,16 +791,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A13:A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="12" width="91.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="13" width="91.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.56"/>
   </cols>
   <sheetData>
@@ -665,7 +808,7 @@
       <c r="A1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>13</v>
       </c>
     </row>
@@ -673,7 +816,7 @@
       <c r="A2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>15</v>
       </c>
     </row>
@@ -681,7 +824,7 @@
       <c r="A3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="15" t="s">
         <v>17</v>
       </c>
     </row>
@@ -689,55 +832,65 @@
       <c r="A4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="12" t="n">
+      <c r="B4" s="13" t="n">
         <v>2017</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="14" t="s">
+    <row r="6" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="14" t="s">
+    <row r="7" customFormat="false" ht="52.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+    <row r="8" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="15" t="s">
+    </row>
+    <row r="9" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="15" t="s">
+    <row r="10" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="B10" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="12" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+    <row r="12" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B12" s="13" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="39.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>